<commit_message>
doc (Rapport/grille) : complétation du rappot et de la grille d'éval
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601B4A75-F171-44B8-8473-0EF969EE04E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305DA60C-FF54-4742-8015-A836E5C36BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Journal de travail'!$A$6:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4126,7 +4127,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10987,6 +10988,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -10996,15 +11006,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11221,6 +11222,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11229,14 +11238,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(JdT/rapport) : ajout du docx et mise a jour du JdT
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\P_ShootMeUp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5D9587-CDF6-4FB0-9CBB-E44574063C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B5671D-367C-4A48-BA5F-C1CA74517A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>compléter lea grille d'éval</t>
+  </si>
+  <si>
+    <t>modification des user story (test dacceptance)</t>
+  </si>
+  <si>
+    <t>j'ai fait  les 12 US</t>
+  </si>
+  <si>
+    <t>US de 1 a 5</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1106,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>275</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4135,7 +4144,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4190,7 +4199,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>4 heures 35 minutes</v>
+        <v>4 heures 45 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4209,11 +4218,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4318,7 +4327,9 @@
       <c r="F9" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="46"/>
+      <c r="G9" s="46" t="s">
+        <v>37</v>
+      </c>
       <c r="M9" t="s">
         <v>19</v>
       </c>
@@ -4390,16 +4401,26 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
+        <v>37</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45910</v>
+      </c>
       <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="45"/>
+      <c r="D12" s="38">
+        <v>10</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>38</v>
+      </c>
       <c r="N12">
         <v>5</v>
       </c>
@@ -10928,11 +10949,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10940,7 +10961,7 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 35 min</v>
+        <v>4 h 45 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
@@ -10965,22 +10986,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 35 min</v>
+        <v>4 h 45 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>5.2083333333333336E-2</v>
+        <v>5.3977272727272728E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Doc(rapport) : correction des objectifs pedagogiques
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B5671D-367C-4A48-BA5F-C1CA74517A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B5D68-32E6-421C-A162-00E0A3635B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -4144,7 +4144,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4429,14 +4429,18 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="str">
+      <c r="A13" s="74">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
+        <v>37</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45910</v>
+      </c>
       <c r="C13" s="41"/>
       <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="E13" s="43" t="s">
+        <v>4</v>
+      </c>
       <c r="F13" s="28"/>
       <c r="G13" s="46"/>
       <c r="N13">
@@ -11045,6 +11049,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11054,15 +11067,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11279,6 +11283,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11287,14 +11299,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat(code) : inportation et modif de l'exemple "Drone"
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B5D68-32E6-421C-A162-00E0A3635B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9972A60D-860D-4264-97C3-66A08DA3B99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Auteur:</t>
   </si>
@@ -157,7 +157,16 @@
     <t>j'ai fait  les 12 US</t>
   </si>
   <si>
-    <t>US de 1 a 5</t>
+    <t>modification du rapport suite au feedback</t>
+  </si>
+  <si>
+    <t>création de l'objet joueur et mouvement</t>
+  </si>
+  <si>
+    <t>US de 6 à</t>
+  </si>
+  <si>
+    <t>US de 1 à 5</t>
   </si>
 </sst>
 </file>
@@ -1100,13 +1109,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>285</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1952,13 +1961,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.12121212121212122</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.87878787878787878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4144,7 +4153,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4208,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>4 heures 45 minutes</v>
+        <v>5 heures 30 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4218,11 +4227,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>285</v>
+        <v>330</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4419,7 +4428,7 @@
         <v>36</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N12">
         <v>5</v>
@@ -4437,11 +4446,15 @@
         <v>45910</v>
       </c>
       <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
+      <c r="D13" s="42">
+        <v>5</v>
+      </c>
       <c r="E13" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="G13" s="46"/>
       <c r="N13">
         <v>6</v>
@@ -4451,15 +4464,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
+        <v>37</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45910</v>
+      </c>
       <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="38">
+        <v>40</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>39</v>
+      </c>
       <c r="G14" s="45"/>
       <c r="N14">
         <v>7</v>
@@ -4469,16 +4490,24 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="str">
+      <c r="A15" s="74">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="40"/>
+        <v>37</v>
+      </c>
+      <c r="B15" s="40">
+        <v>45910</v>
+      </c>
       <c r="C15" s="41"/>
       <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="46"/>
+      <c r="E15" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>40</v>
+      </c>
       <c r="N15">
         <v>8</v>
       </c>
@@ -10879,11 +10908,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10891,11 +10920,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>0 h 40 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10953,11 +10982,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10965,11 +10994,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 45 min</v>
+        <v>4 h 50 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.87878787878787878</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10990,22 +11019,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>285</v>
+        <v>330</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 45 min</v>
+        <v>5 h 30 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>5.3977272727272728E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11049,15 +11078,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11067,6 +11087,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11283,14 +11312,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11299,6 +11320,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Doc(JDT) : complété le jdt du 10.09.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9972A60D-860D-4264-97C3-66A08DA3B99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEA8C6F-2E9F-4FE5-815D-98FE800CFBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Auteur:</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>US de 1 à 5</t>
+  </si>
+  <si>
+    <t>importation et modif de l'exemple "Drone"</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>continuation des mouvement</t>
   </si>
 </sst>
 </file>
@@ -1109,13 +1118,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>290</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1961,13 +1970,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12121212121212122</c:v>
+                  <c:v>0.24691358024691357</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87878787878787878</c:v>
+                  <c:v>0.75308641975308643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4153,7 +4162,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4208,7 +4217,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 30 minutes</v>
+        <v>6 heures 45 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4227,11 +4236,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>330</v>
+        <v>405</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4481,7 +4490,9 @@
       <c r="F14" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="N14">
         <v>7</v>
       </c>
@@ -4498,7 +4509,9 @@
         <v>45910</v>
       </c>
       <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
+      <c r="D15" s="42">
+        <v>15</v>
+      </c>
       <c r="E15" s="43" t="s">
         <v>4</v>
       </c>
@@ -4516,31 +4529,49 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="73" t="str">
+      <c r="A16" s="73">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="36"/>
+        <v>37</v>
+      </c>
+      <c r="B16" s="36">
+        <v>45910</v>
+      </c>
       <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="38">
+        <v>35</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="G16" s="45"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="str">
+      <c r="A17" s="74">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="40"/>
+        <v>37</v>
+      </c>
+      <c r="B17" s="40">
+        <v>45910</v>
+      </c>
       <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="46"/>
+      <c r="D17" s="42">
+        <v>25</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>43</v>
+      </c>
       <c r="O17">
         <v>45</v>
       </c>
@@ -10908,11 +10939,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10920,11 +10951,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 40 min</v>
+        <v>1 h 40 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.12121212121212122</v>
+        <v>0.24691358024691357</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10982,11 +11013,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10994,11 +11025,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 50 min</v>
+        <v>5 h 05 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.87878787878787878</v>
+        <v>0.75308641975308643</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11019,22 +11050,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>330</v>
+        <v>405</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 30 min</v>
+        <v>6 h 45 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>6.25E-2</v>
+        <v>7.6704545454545456E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Doc(jdt) :compléter jdt du 17.09.25
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEA8C6F-2E9F-4FE5-815D-98FE800CFBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C9A4DD-55CF-4521-AF25-670BC3787FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Auteur:</t>
   </si>
@@ -176,6 +176,27 @@
   </si>
   <si>
     <t>continuation des mouvement</t>
+  </si>
+  <si>
+    <t>ajustement des direction et test des mouvement (console)</t>
+  </si>
+  <si>
+    <t>préparation des image pour le joueur</t>
+  </si>
+  <si>
+    <t>passage des mouvement par console &gt; rendu graphique</t>
+  </si>
+  <si>
+    <t>problème de visibilité des issues</t>
+  </si>
+  <si>
+    <t>passage des mouvement par console &gt; rendu graphique FIN</t>
+  </si>
+  <si>
+    <t>création des block</t>
+  </si>
+  <si>
+    <t>wip</t>
   </si>
 </sst>
 </file>
@@ -1118,13 +1139,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>305</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,13 +1991,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24691358024691357</c:v>
+                  <c:v>0.46218487394957986</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75308641975308643</c:v>
+                  <c:v>0.53781512605042014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4162,7 +4183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4217,7 +4238,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 45 minutes</v>
+        <v>9 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4232,15 +4253,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>225</v>
+        <v>355</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>405</v>
+        <v>595</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4577,82 +4598,136 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="str">
+      <c r="A18" s="73">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="B18" s="36">
+        <v>45917</v>
+      </c>
       <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="28"/>
+      <c r="D18" s="38">
+        <v>20</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>45</v>
+      </c>
       <c r="G18" s="45"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="str">
+      <c r="A19" s="74">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="B19" s="40">
+        <v>45917</v>
+      </c>
       <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="28"/>
+      <c r="D19" s="42">
+        <v>10</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" s="46"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="str">
+      <c r="A20" s="73">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="B20" s="36">
+        <v>45917</v>
+      </c>
       <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="45"/>
+      <c r="D20" s="38">
+        <v>50</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="str">
+      <c r="A21" s="74">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="B21" s="40">
+        <v>45917</v>
+      </c>
       <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="28"/>
+      <c r="D21" s="42">
+        <v>15</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="G21" s="46"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="str">
+      <c r="A22" s="73">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="B22" s="36">
+        <v>45917</v>
+      </c>
       <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="28"/>
+      <c r="D22" s="38">
+        <v>20</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="str">
+      <c r="A23" s="74">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="46"/>
+        <v>38</v>
+      </c>
+      <c r="B23" s="40">
+        <v>45917</v>
+      </c>
+      <c r="C23" s="41">
+        <v>1</v>
+      </c>
+      <c r="D23" s="42">
+        <v>15</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="str">
@@ -10935,15 +11010,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>215</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>275</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10951,11 +11026,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>1 h 40 min</v>
+        <v>4 h 35 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.24691358024691357</v>
+        <v>0.46218487394957986</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11013,11 +11088,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11025,11 +11100,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 05 min</v>
+        <v>5 h 20 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.75308641975308643</v>
+        <v>0.53781512605042014</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11046,26 +11121,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>225</v>
+        <v>355</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>405</v>
+        <v>595</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 45 min</v>
+        <v>9 h 55 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>7.6704545454545456E-2</v>
+        <v>0.11268939393939394</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11109,6 +11184,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11118,15 +11202,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11343,6 +11418,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11351,14 +11434,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(jdt) : jdt du 24.09.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C9A4DD-55CF-4521-AF25-670BC3787FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3141036E-F8D1-4219-B917-7D3ADF91B951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Auteur:</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>wip</t>
+  </si>
+  <si>
+    <t>modification de l'image des block</t>
+  </si>
+  <si>
+    <t>rotation des block</t>
+  </si>
+  <si>
+    <t>création des hitbox des block</t>
+  </si>
+  <si>
+    <t>Rotation des block</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1148,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1988,16 +2000,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.16774193548387098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46218487394957986</c:v>
+                  <c:v>0.41935483870967744</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53781512605042014</c:v>
+                  <c:v>0.41290322580645161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4183,7 +4195,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4238,7 +4250,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 55 minutes</v>
+        <v>12 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4253,15 +4265,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>355</v>
+        <v>415</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>595</v>
+        <v>775</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4730,52 +4742,90 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="str">
+      <c r="A24" s="73">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="36"/>
+        <v>39</v>
+      </c>
+      <c r="B24" s="36">
+        <v>45924</v>
+      </c>
       <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="28"/>
+      <c r="D24" s="38">
+        <v>25</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="str">
+      <c r="A25" s="74">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="46"/>
+        <v>39</v>
+      </c>
+      <c r="B25" s="40">
+        <v>45924</v>
+      </c>
+      <c r="C25" s="41">
+        <v>1</v>
+      </c>
+      <c r="D25" s="42">
+        <v>10</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="73" t="str">
+      <c r="A26" s="73">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+        <v>39</v>
+      </c>
+      <c r="B26" s="36">
+        <v>45924</v>
+      </c>
+      <c r="C26" s="37">
+        <v>1</v>
+      </c>
       <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="28"/>
+      <c r="E26" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="str">
+      <c r="A27" s="74">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="40"/>
+        <v>39</v>
+      </c>
+      <c r="B27" s="40">
+        <v>45924</v>
+      </c>
       <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="46"/>
+      <c r="D27" s="42">
+        <v>25</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="46" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="73" t="str">
@@ -10973,15 +11023,15 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10989,11 +11039,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>2 h 10 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0</v>
+        <v>0.16774193548387098</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11014,11 +11064,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11026,11 +11076,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 35 min</v>
+        <v>5 h 25 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.46218487394957986</v>
+        <v>0.41935483870967744</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11104,7 +11154,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.53781512605042014</v>
+        <v>0.41290322580645161</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11121,26 +11171,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>355</v>
+        <v>415</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>595</v>
+        <v>775</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 55 min</v>
+        <v>12 h 55 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.11268939393939394</v>
+        <v>0.14678030303030304</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11184,15 +11234,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11202,6 +11243,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11418,14 +11468,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11434,6 +11476,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Doc(jdt) : complété le jdt pour le 01.10.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBFF584-3869-4915-8D25-B743BDB42207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ACE5A5-E988-487C-913D-D4750A729119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>Auteur:</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>Rotation des block</t>
+  </si>
+  <si>
+    <t>tir du joueur</t>
+  </si>
+  <si>
+    <t>mise de la rotation dans le model et prrograme (WIP)</t>
+  </si>
+  <si>
+    <t>Créeation de la class bullet avec la touche d'activation et création lors du click gauche (wip)</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1160,7 @@
                   <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>325</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2000,16 +2009,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.16774193548387098</c:v>
+                  <c:v>0.14054054054054055</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41935483870967744</c:v>
+                  <c:v>0.51351351351351349</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41290322580645161</c:v>
+                  <c:v>0.34594594594594597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4250,7 +4259,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>12 heures 55 minutes</v>
+        <v>15 heures 25 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4265,15 +4274,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>415</v>
+        <v>445</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>775</v>
+        <v>925</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4827,29 +4836,53 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="str">
+    <row r="28" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="73">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="45"/>
+        <v>40</v>
+      </c>
+      <c r="B28" s="36">
+        <v>45931</v>
+      </c>
+      <c r="C28" s="37">
+        <v>1</v>
+      </c>
+      <c r="D28" s="38">
+        <v>10</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="str">
+      <c r="A29" s="74">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="46"/>
+        <v>40</v>
+      </c>
+      <c r="B29" s="40">
+        <v>45931</v>
+      </c>
+      <c r="C29" s="41">
+        <v>1</v>
+      </c>
+      <c r="D29" s="42">
+        <v>20</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="46" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="73" t="str">
@@ -11043,7 +11076,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.16774193548387098</v>
+        <v>0.14054054054054055</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11060,15 +11093,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>265</v>
+        <v>295</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>475</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11076,11 +11109,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>5 h 25 min</v>
+        <v>7 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.41935483870967744</v>
+        <v>0.51351351351351349</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11154,7 +11187,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.41290322580645161</v>
+        <v>0.34594594594594597</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11171,26 +11204,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>415</v>
+        <v>445</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>775</v>
+        <v>925</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>12 h 55 min</v>
+        <v>15 h 25 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.14678030303030304</v>
+        <v>0.17518939393939395</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11234,6 +11267,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11243,15 +11285,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11468,6 +11501,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11476,14 +11517,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Doc(jdt) jdt du 03.10.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ACE5A5-E988-487C-913D-D4750A729119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DF4ACB-D80C-4BA5-83F1-1C3316A4A669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Auteur:</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Créeation de la class bullet avec la touche d'activation et création lors du click gauche (wip)</t>
+  </si>
+  <si>
+    <t>Rapport (UML)</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1169,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>320</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2009,16 +2012,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.14054054054054055</c:v>
+                  <c:v>0.13829787234042554</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51351351351351349</c:v>
+                  <c:v>0.50531914893617025</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34594594594594597</c:v>
+                  <c:v>0.35638297872340424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4204,7 +4207,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4259,7 +4262,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>15 heures 25 minutes</v>
+        <v>15 heures 40 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4278,11 +4281,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>925</v>
+        <v>940</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4885,16 +4888,26 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="str">
+      <c r="A30" s="73">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="36"/>
+        <v>40</v>
+      </c>
+      <c r="B30" s="36">
+        <v>45933</v>
+      </c>
       <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="45"/>
+      <c r="D30" s="38">
+        <v>15</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="str">
@@ -11076,7 +11089,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.14054054054054055</v>
+        <v>0.13829787234042554</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11113,7 +11126,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.51351351351351349</v>
+        <v>0.50531914893617025</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11171,11 +11184,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11183,11 +11196,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 20 min</v>
+        <v>5 h 35 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.34594594594594597</v>
+        <v>0.35638297872340424</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11208,22 +11221,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>925</v>
+        <v>940</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>15 h 25 min</v>
+        <v>15 h 40 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.17518939393939395</v>
+        <v>0.17803030303030304</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11267,15 +11280,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11285,6 +11289,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11501,14 +11514,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11517,6 +11522,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Doc(jdt/rapport) : jdt du 08.10.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\I320\Local repo\Big-Nightmare\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\Github\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DF4ACB-D80C-4BA5-83F1-1C3316A4A669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FC4AD8-B37F-4330-AED6-5470746494AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>Auteur:</t>
   </si>
@@ -221,6 +221,15 @@
   </si>
   <si>
     <t>Rapport (UML)</t>
+  </si>
+  <si>
+    <t>supression de la rotation des block et mise en image</t>
+  </si>
+  <si>
+    <t>fonctionenemt des hitbox block</t>
+  </si>
+  <si>
+    <t>ajout des images des mobs</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1169,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>130</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>475</c:v>
+                  <c:v>595</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2012,16 +2021,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.13829787234042554</c:v>
+                  <c:v>0.14678899082568808</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50531914893617025</c:v>
+                  <c:v>0.54587155963302747</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35638297872340424</c:v>
+                  <c:v>0.30733944954128439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4206,8 +4215,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4262,7 +4271,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>15 heures 40 minutes</v>
+        <v>18 heures 10 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4277,15 +4286,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>460</v>
+        <v>550</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>940</v>
+        <v>1090</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4910,51 +4919,85 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="str">
+      <c r="A31" s="74">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="B31" s="40">
+        <v>45938</v>
+      </c>
+      <c r="C31" s="41">
+        <v>1</v>
+      </c>
+      <c r="D31" s="42">
+        <v>55</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="G31" s="46"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="73" t="str">
+      <c r="A32" s="73">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="36"/>
+        <v>41</v>
+      </c>
+      <c r="B32" s="36">
+        <v>45938</v>
+      </c>
       <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="28"/>
+      <c r="D32" s="38">
+        <v>20</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="G32" s="45"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="str">
+      <c r="A33" s="74">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="40"/>
+        <v>41</v>
+      </c>
+      <c r="B33" s="40">
+        <v>45938</v>
+      </c>
       <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="27"/>
+      <c r="D33" s="42">
+        <v>5</v>
+      </c>
+      <c r="E33" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>62</v>
+      </c>
       <c r="G33" s="46"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="73" t="str">
+      <c r="A34" s="73">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="36"/>
+        <v>41</v>
+      </c>
+      <c r="B34" s="36">
+        <v>45938</v>
+      </c>
       <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="27"/>
+      <c r="D34" s="38">
+        <v>10</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>61</v>
+      </c>
       <c r="G34" s="45"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -11073,11 +11116,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11085,11 +11128,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>2 h 10 min</v>
+        <v>2 h 40 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.13829787234042554</v>
+        <v>0.14678899082568808</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11106,15 +11149,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>295</v>
+        <v>355</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>475</v>
+        <v>595</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11122,11 +11165,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>7 h 55 min</v>
+        <v>9 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.50531914893617025</v>
+        <v>0.54587155963302747</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11200,7 +11243,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.35638297872340424</v>
+        <v>0.30733944954128439</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11217,26 +11260,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>460</v>
+        <v>550</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>940</v>
+        <v>1090</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>15 h 40 min</v>
+        <v>18 h 10 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.17803030303030304</v>
+        <v>0.20643939393939395</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
doc(jdt) jdt du 28.10.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\Github\Big-Nightmare\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FC4AD8-B37F-4330-AED6-5470746494AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2AD069-C6E9-4D9E-AF2F-2FD54A840C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>Auteur:</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>ajout des images des mobs</t>
+  </si>
+  <si>
+    <t>collision entre le player et les block</t>
+  </si>
+  <si>
+    <t>hitbox player/block et collision</t>
+  </si>
+  <si>
+    <t>création des classe mobRed et mobYellow</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1181,7 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>595</c:v>
+                  <c:v>795</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2021,16 +2030,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.14678899082568808</c:v>
+                  <c:v>0.12403100775193798</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54587155963302747</c:v>
+                  <c:v>0.61627906976744184</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30733944954128439</c:v>
+                  <c:v>0.25968992248062017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4215,8 +4224,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4271,7 +4280,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>18 heures 10 minutes</v>
+        <v>21 heures 30 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4286,15 +4295,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>720</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1090</v>
+        <v>1290</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5001,40 +5010,68 @@
       <c r="G34" s="45"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="74" t="str">
+      <c r="A35" s="74">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
+        <v>44</v>
+      </c>
+      <c r="B35" s="40">
+        <v>45958</v>
+      </c>
+      <c r="C35" s="41">
+        <v>2</v>
+      </c>
       <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="46"/>
+      <c r="E35" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="46" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="73" t="str">
+      <c r="A36" s="73">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
+        <v>44</v>
+      </c>
+      <c r="B36" s="36">
+        <v>45958</v>
+      </c>
+      <c r="C36" s="37">
+        <v>1</v>
+      </c>
       <c r="D36" s="38"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>56</v>
+      </c>
       <c r="G36" s="45"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="74" t="str">
+      <c r="A37" s="74">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B37" s="40">
+        <v>45958</v>
+      </c>
       <c r="C37" s="41"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="46"/>
+      <c r="D37" s="42">
+        <v>20</v>
+      </c>
+      <c r="E37" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="46" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="73" t="str">
@@ -11132,7 +11169,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.14678899082568808</v>
+        <v>0.12403100775193798</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11149,15 +11186,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>420</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>595</v>
+        <v>795</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11165,11 +11202,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>9 h 55 min</v>
+        <v>13 h 15 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.54587155963302747</v>
+        <v>0.61627906976744184</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11243,7 +11280,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.30733944954128439</v>
+        <v>0.25968992248062017</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11260,26 +11297,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>540</v>
+        <v>720</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1090</v>
+        <v>1290</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>18 h 10 min</v>
+        <v>21 h 30 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.20643939393939395</v>
+        <v>0.24431818181818182</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11323,6 +11360,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11332,15 +11378,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11557,6 +11594,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11565,14 +11610,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(jdt) jdt du 29.10.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\Big-Nightmare\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\Github\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2AD069-C6E9-4D9E-AF2F-2FD54A840C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F71B06-96EA-4447-BBCC-F6C98A1C70D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>Auteur:</t>
   </si>
@@ -239,6 +239,18 @@
   </si>
   <si>
     <t>création des classe mobRed et mobYellow</t>
+  </si>
+  <si>
+    <t>modification de la création de circle hitbox et position de départ du joueur</t>
+  </si>
+  <si>
+    <t>création des mob</t>
+  </si>
+  <si>
+    <t>génération de position aléatoire</t>
+  </si>
+  <si>
+    <t>mort des mob quand les pv tombes a 0 ou moins</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1193,7 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>795</c:v>
+                  <c:v>985</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2030,16 +2042,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.12403100775193798</c:v>
+                  <c:v>0.10810810810810811</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61627906976744184</c:v>
+                  <c:v>0.66554054054054057</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25968992248062017</c:v>
+                  <c:v>0.22635135135135134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4224,8 +4236,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4280,7 +4292,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>21 heures 30 minutes</v>
+        <v>24 heures 40 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4295,15 +4307,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>720</v>
+        <v>780</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>570</v>
+        <v>700</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1290</v>
+        <v>1480</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5074,40 +5086,70 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="73" t="str">
+      <c r="A38" s="73">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="36"/>
+        <v>44</v>
+      </c>
+      <c r="B38" s="36">
+        <v>45959</v>
+      </c>
       <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="27"/>
+      <c r="D38" s="38">
+        <v>35</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>66</v>
+      </c>
       <c r="G38" s="45"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="74" t="str">
+      <c r="A39" s="74">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="46"/>
+        <v>44</v>
+      </c>
+      <c r="B39" s="40">
+        <v>45959</v>
+      </c>
+      <c r="C39" s="41">
+        <v>1</v>
+      </c>
+      <c r="D39" s="42">
+        <v>50</v>
+      </c>
+      <c r="E39" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G39" s="46" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="73" t="str">
+      <c r="A40" s="73">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="36"/>
+        <v>44</v>
+      </c>
+      <c r="B40" s="36">
+        <v>45959</v>
+      </c>
       <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="45"/>
+      <c r="D40" s="38">
+        <v>45</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="74" t="str">
@@ -11169,7 +11211,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.12403100775193798</v>
+        <v>0.10810810810810811</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11186,15 +11228,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>375</v>
+        <v>505</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>795</v>
+        <v>985</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11202,11 +11244,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>13 h 15 min</v>
+        <v>16 h 25 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.61627906976744184</v>
+        <v>0.66554054054054057</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11280,7 +11322,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.25968992248062017</v>
+        <v>0.22635135135135134</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11297,26 +11339,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>720</v>
+        <v>780</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>570</v>
+        <v>700</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1290</v>
+        <v>1480</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>21 h 30 min</v>
+        <v>24 h 40 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.24431818181818182</v>
+        <v>0.28030303030303028</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11360,15 +11402,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11378,6 +11411,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11594,14 +11636,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11610,6 +11644,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Doc(jdt) jdt du 31.10.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\Github\Big-Nightmare\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F71B06-96EA-4447-BBCC-F6C98A1C70D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Auteur:</t>
   </si>
@@ -1199,7 +1199,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>335</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2042,16 +2042,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.10810810810810811</c:v>
+                  <c:v>0.10666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66554054054054057</c:v>
+                  <c:v>0.65666666666666662</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22635135135135134</c:v>
+                  <c:v>0.23666666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4237,7 +4237,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4292,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>24 heures 40 minutes</v>
+        <v>25 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4311,11 +4311,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1480</v>
+        <v>1500</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5152,15 +5152,23 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="74" t="str">
+      <c r="A41" s="74">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B41" s="40">
+        <v>45961</v>
+      </c>
       <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="27"/>
+      <c r="D41" s="42">
+        <v>20</v>
+      </c>
+      <c r="E41" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>59</v>
+      </c>
       <c r="G41" s="46"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -11211,7 +11219,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.10810810810810811</v>
+        <v>0.10666666666666667</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11248,7 +11256,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.66554054054054057</v>
+        <v>0.65666666666666662</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11306,11 +11314,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11318,11 +11326,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 35 min</v>
+        <v>5 h 55 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.22635135135135134</v>
+        <v>0.23666666666666666</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11343,22 +11351,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1480</v>
+        <v>1500</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>24 h 40 min</v>
+        <v>25 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.28030303030303028</v>
+        <v>0.28409090909090912</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11402,6 +11410,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11411,15 +11428,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11636,6 +11644,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11644,14 +11660,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOC(jdt) jdt du 01.11.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\Github\Big-Nightmare\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bec7660434da09f6/Documents/github/Big-Nightmare/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4304A3E6-A8C6-40F0-B175-CBEE17545DF4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="585" yWindow="1695" windowWidth="22980" windowHeight="12060" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Auteur:</t>
   </si>
@@ -251,6 +251,21 @@
   </si>
   <si>
     <t>mort des mob quand les pv tombes a 0 ou moins</t>
+  </si>
+  <si>
+    <t>les MobRed vont vers le joueur</t>
+  </si>
+  <si>
+    <t>diminution du temps entre les tire des MonYellow</t>
+  </si>
+  <si>
+    <t>les MobRed sont bloquer par les block</t>
+  </si>
+  <si>
+    <t>ajout des pv des block et changement de couleur</t>
+  </si>
+  <si>
+    <t>ajout des dégat des mobs au player et au block</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1208,7 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>985</c:v>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1263,6 +1278,7 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1270,7 +1286,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1610,6 +1625,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1617,7 +1633,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2042,16 +2057,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.10666666666666667</c:v>
+                  <c:v>8.6253369272237201E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65666666666666662</c:v>
+                  <c:v>0.72237196765498657</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23666666666666666</c:v>
+                  <c:v>0.19137466307277629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,6 +2221,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2213,7 +2229,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4029,6 +4044,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
@@ -4235,9 +4254,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4311,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>25 heures 0 minutes</v>
+        <v>30 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4307,15 +4326,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>780</v>
+        <v>1020</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>720</v>
+        <v>835</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1500</v>
+        <v>1855</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5172,88 +5191,152 @@
       <c r="G41" s="46"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="73" t="str">
+      <c r="A42" s="73">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="36"/>
+        <v>44</v>
+      </c>
+      <c r="B42" s="36">
+        <v>45962</v>
+      </c>
       <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="27"/>
+      <c r="D42" s="38">
+        <v>30</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="G42" s="45"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="74" t="str">
+      <c r="A43" s="74">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B43" s="40">
+        <v>45962</v>
+      </c>
       <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="27"/>
+      <c r="D43" s="42">
+        <v>10</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>70</v>
+      </c>
       <c r="G43" s="46"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="73" t="str">
+      <c r="A44" s="73">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="36"/>
+        <v>44</v>
+      </c>
+      <c r="B44" s="36">
+        <v>45962</v>
+      </c>
       <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="27"/>
+      <c r="D44" s="38">
+        <v>10</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>71</v>
+      </c>
       <c r="G44" s="45"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="74" t="str">
+      <c r="A45" s="74">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="40">
+        <v>45962</v>
+      </c>
       <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="27"/>
+      <c r="D45" s="42">
+        <v>15</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>72</v>
+      </c>
       <c r="G45" s="46"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="73" t="str">
+      <c r="A46" s="73">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="36">
+        <v>45962</v>
+      </c>
+      <c r="C46" s="37">
+        <v>1</v>
+      </c>
       <c r="D46" s="38"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="27"/>
+      <c r="E46" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>73</v>
+      </c>
       <c r="G46" s="45"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="74" t="str">
+      <c r="A47" s="74">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="46"/>
+        <v>44</v>
+      </c>
+      <c r="B47" s="40">
+        <v>45962</v>
+      </c>
+      <c r="C47" s="41">
+        <v>1</v>
+      </c>
+      <c r="D47" s="42">
+        <v>30</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="46" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="73">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="36"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="45"/>
+        <v>44</v>
+      </c>
+      <c r="B48" s="36">
+        <v>45962</v>
+      </c>
+      <c r="C48" s="37">
+        <v>2</v>
+      </c>
+      <c r="D48" s="38">
+        <v>20</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="45" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="str">
@@ -11219,7 +11302,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.10666666666666667</v>
+        <v>8.6253369272237201E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11236,15 +11319,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>505</v>
+        <v>620</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>985</v>
+        <v>1340</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11252,11 +11335,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>16 h 25 min</v>
+        <v>22 h 20 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.65666666666666662</v>
+        <v>0.72237196765498657</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11330,7 +11413,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.23666666666666666</v>
+        <v>0.19137466307277629</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11347,26 +11430,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>780</v>
+        <v>1020</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>720</v>
+        <v>835</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1500</v>
+        <v>1855</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>25 h 00 min</v>
+        <v>30 h 55 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.28409090909090912</v>
+        <v>0.35132575757575757</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Doc(jdt) jdt : 01.11.2025 partie 2
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bec7660434da09f6/Documents/github/Big-Nightmare/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4304A3E6-A8C6-40F0-B175-CBEE17545DF4}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47C8C84E-1D5F-4CD7-AF04-3485F3B7605D}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="1695" windowWidth="22980" windowHeight="12060" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>Auteur:</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>ajout des dégat des mobs au player et au block</t>
+  </si>
+  <si>
+    <t>ajout du scord qui augment</t>
+  </si>
+  <si>
+    <t>Rapport</t>
   </si>
 </sst>
 </file>
@@ -1208,13 +1214,13 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1340</c:v>
+                  <c:v>1380</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>355</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2057,16 +2063,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.6253369272237201E-2</c:v>
+                  <c:v>8.1841432225063945E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72237196765498657</c:v>
+                  <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19137466307277629</c:v>
+                  <c:v>0.21227621483375958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4254,9 +4260,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4311,7 +4317,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>30 heures 55 minutes</v>
+        <v>32 heures 35 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4326,15 +4332,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1020</v>
+        <v>1080</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>835</v>
+        <v>875</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1855</v>
+        <v>1955</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5339,27 +5345,43 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="74" t="str">
+      <c r="A49" s="74">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v/>
-      </c>
-      <c r="B49" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="40">
+        <v>45962</v>
+      </c>
       <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="27"/>
+      <c r="D49" s="42">
+        <v>40</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="G49" s="46"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="73" t="str">
+      <c r="A50" s="73">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v/>
-      </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+        <v>44</v>
+      </c>
+      <c r="B50" s="36">
+        <v>45962</v>
+      </c>
+      <c r="C50" s="37">
+        <v>1</v>
+      </c>
       <c r="D50" s="38"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="27"/>
+      <c r="E50" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>76</v>
+      </c>
       <c r="G50" s="45"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -11302,7 +11324,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>8.6253369272237201E-2</v>
+        <v>8.1841432225063945E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11323,11 +11345,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>620</v>
+        <v>660</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1340</v>
+        <v>1380</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11335,11 +11357,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>22 h 20 min</v>
+        <v>23 h 00 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.72237196765498657</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11393,7 +11415,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
@@ -11401,7 +11423,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>415</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11409,11 +11431,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 55 min</v>
+        <v>6 h 55 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.19137466307277629</v>
+        <v>0.21227621483375958</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11430,26 +11452,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>1020</v>
+        <v>1080</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>835</v>
+        <v>875</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1855</v>
+        <v>1955</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>30 h 55 min</v>
+        <v>32 h 35 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.35132575757575757</v>
+        <v>0.37026515151515149</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11493,15 +11515,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11511,6 +11524,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11727,14 +11749,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11743,6 +11757,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOC (jdt) jdt du 8.11.2025
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Doc/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bec7660434da09f6/Documents/github/Big-Nightmare/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47C8C84E-1D5F-4CD7-AF04-3485F3B7605D}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{1B6BF7D0-C1ED-41B5-96F0-5851E980C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68940BB2-1A15-4F48-BC94-151EB75C6F79}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="1695" windowWidth="22980" windowHeight="12060" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
   <si>
     <t>Auteur:</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Rapport</t>
+  </si>
+  <si>
+    <t>17h20</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1223,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>415</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2063,16 +2066,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.1841432225063945E-2</c:v>
+                  <c:v>8.0200501253132828E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70588235294117652</c:v>
+                  <c:v>0.69172932330827064</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.21227621483375958</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4257,12 +4260,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF2E8F1-C793-7E43-B3DE-C075053A97DA}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4317,7 +4322,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>32 heures 35 minutes</v>
+        <v>33 heures 15 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4336,11 +4341,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>875</v>
+        <v>915</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1955</v>
+        <v>1995</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5385,16 +5390,26 @@
       <c r="G50" s="45"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="74" t="str">
+      <c r="A51" s="74">
         <f>IF(ISBLANK(B51),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B51))</f>
-        <v/>
-      </c>
-      <c r="B51" s="40"/>
+        <v>45</v>
+      </c>
+      <c r="B51" s="40">
+        <v>45969</v>
+      </c>
       <c r="C51" s="41"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="46"/>
+      <c r="D51" s="42">
+        <v>40</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51" s="46" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="73" t="str">
@@ -11213,8 +11228,8 @@
       <formula1>$M$7:$M$11</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -11324,7 +11339,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>8.1841432225063945E-2</v>
+        <v>8.0200501253132828E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11361,7 +11376,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.70588235294117652</v>
+        <v>0.69172932330827064</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11419,11 +11434,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>415</v>
+        <v>455</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11431,11 +11446,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 55 min</v>
+        <v>7 h 35 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.21227621483375958</v>
+        <v>0.22807017543859648</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11456,22 +11471,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>875</v>
+        <v>915</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1955</v>
+        <v>1995</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>32 h 35 min</v>
+        <v>33 h 15 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.37026515151515149</v>
+        <v>0.37784090909090912</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11527,15 +11542,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="020ab319e6f8d23aec07c29d6516d4ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e15d3f914bf2a775f9387e5284d9197" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11748,6 +11754,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
@@ -11762,14 +11777,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11786,4 +11793,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>